<commit_message>
I modified rows 2 and 5 to have decimal values.
</commit_message>
<xml_diff>
--- a/2025/24_Agro_24.xlsx
+++ b/2025/24_Agro_24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\24-AGR-24\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0BC480-5A52-4C0A-A87A-6F97AF289C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352C70B1-259A-4F41-B913-78959C301D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{270B01E8-BC1B-48F2-A63B-1CB23688CFEC}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3266" uniqueCount="1363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3266" uniqueCount="1364">
   <si>
     <t>title</t>
   </si>
@@ -4109,6 +4109,9 @@
   </si>
   <si>
     <t>SELECT LEFT(CASE WHEN TRIM(c.code) REGEXP '^[135]' AND CHAR_LENGTH(TRIM(c.code)) = 6 THEN CONCAT('0', TRIM(c.code)) ELSE TRIM(c.code) END , 7) AS code, CONCAT(LEFT(CASE WHEN TRIM(c.code) REGEXP '^[135]' AND CHAR_LENGTH(TRIM(c.code)) = 6 THEN CONCAT('0', TRIM(c.code)) ELSE TRIM(c.code) END, 7), ' - ',  t.name) FROM taxonomy_term_data t JOIN classifier_cuatm_full c ON c.tid = t.tid  WHERE c.prgs in ('2') AND c.code not in ('0000000','1111111','2222222','3333333');</t>
+  </si>
+  <si>
+    <t>float</t>
   </si>
 </sst>
 </file>
@@ -4505,15 +4508,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8135B143-8B24-45DC-A0A8-6A34CB095E14}">
   <dimension ref="A1:AH497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F269" sqref="F269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
@@ -5946,7 +5949,7 @@
         <v>184</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G22" t="s">
         <v>33</v>
@@ -5991,7 +5994,7 @@
         <v>100</v>
       </c>
       <c r="Z22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB22">
         <v>0</v>
@@ -6008,7 +6011,7 @@
         <v>185</v>
       </c>
       <c r="F23" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G23" t="s">
         <v>33</v>
@@ -6053,7 +6056,7 @@
         <v>100</v>
       </c>
       <c r="Z23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB23">
         <v>0</v>
@@ -6070,7 +6073,7 @@
         <v>186</v>
       </c>
       <c r="F24" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
@@ -6115,7 +6118,7 @@
         <v>100</v>
       </c>
       <c r="Z24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB24">
         <v>0</v>
@@ -6132,7 +6135,7 @@
         <v>187</v>
       </c>
       <c r="F25" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G25" t="s">
         <v>33</v>
@@ -6177,7 +6180,7 @@
         <v>100</v>
       </c>
       <c r="Z25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB25">
         <v>0</v>
@@ -6194,7 +6197,7 @@
         <v>188</v>
       </c>
       <c r="F26" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G26" t="s">
         <v>33</v>
@@ -6239,7 +6242,7 @@
         <v>100</v>
       </c>
       <c r="Z26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB26">
         <v>0</v>
@@ -6256,7 +6259,7 @@
         <v>191</v>
       </c>
       <c r="F27" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G27" t="s">
         <v>33</v>
@@ -6301,7 +6304,7 @@
         <v>100</v>
       </c>
       <c r="Z27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB27">
         <v>0</v>
@@ -7124,7 +7127,7 @@
         <v>205</v>
       </c>
       <c r="F41" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G41" t="s">
         <v>33</v>
@@ -7169,7 +7172,7 @@
         <v>100</v>
       </c>
       <c r="Z41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB41">
         <v>0</v>
@@ -7186,7 +7189,7 @@
         <v>206</v>
       </c>
       <c r="F42" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G42" t="s">
         <v>33</v>
@@ -7231,7 +7234,7 @@
         <v>100</v>
       </c>
       <c r="Z42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB42">
         <v>0</v>
@@ -7248,7 +7251,7 @@
         <v>207</v>
       </c>
       <c r="F43" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G43" t="s">
         <v>33</v>
@@ -7293,7 +7296,7 @@
         <v>100</v>
       </c>
       <c r="Z43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB43">
         <v>0</v>
@@ -7310,7 +7313,7 @@
         <v>208</v>
       </c>
       <c r="F44" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G44" t="s">
         <v>33</v>
@@ -7355,7 +7358,7 @@
         <v>100</v>
       </c>
       <c r="Z44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB44">
         <v>0</v>
@@ -7372,7 +7375,7 @@
         <v>209</v>
       </c>
       <c r="F45" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G45" t="s">
         <v>33</v>
@@ -7417,7 +7420,7 @@
         <v>100</v>
       </c>
       <c r="Z45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB45">
         <v>0</v>
@@ -7434,7 +7437,7 @@
         <v>210</v>
       </c>
       <c r="F46" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G46" t="s">
         <v>33</v>
@@ -7479,7 +7482,7 @@
         <v>100</v>
       </c>
       <c r="Z46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB46">
         <v>0</v>
@@ -21035,7 +21038,7 @@
         <v>94</v>
       </c>
       <c r="F264" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G264" t="s">
         <v>33</v>
@@ -21080,7 +21083,7 @@
         <v>100</v>
       </c>
       <c r="Z264">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB264">
         <v>0</v>
@@ -21100,7 +21103,7 @@
         <v>94</v>
       </c>
       <c r="F265" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G265" t="s">
         <v>33</v>
@@ -21145,7 +21148,7 @@
         <v>100</v>
       </c>
       <c r="Z265">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB265">
         <v>0</v>
@@ -21165,7 +21168,7 @@
         <v>94</v>
       </c>
       <c r="F266" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G266" t="s">
         <v>33</v>
@@ -21210,7 +21213,7 @@
         <v>100</v>
       </c>
       <c r="Z266">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB266">
         <v>0</v>
@@ -21230,7 +21233,7 @@
         <v>94</v>
       </c>
       <c r="F267" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G267" t="s">
         <v>33</v>
@@ -21275,7 +21278,7 @@
         <v>100</v>
       </c>
       <c r="Z267">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB267">
         <v>0</v>
@@ -21295,7 +21298,7 @@
         <v>94</v>
       </c>
       <c r="F268" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G268" t="s">
         <v>33</v>
@@ -21340,7 +21343,7 @@
         <v>100</v>
       </c>
       <c r="Z268">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB268">
         <v>0</v>
@@ -21360,7 +21363,7 @@
         <v>94</v>
       </c>
       <c r="F269" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G269" t="s">
         <v>33</v>
@@ -21405,7 +21408,7 @@
         <v>100</v>
       </c>
       <c r="Z269">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB269">
         <v>0</v>
@@ -22270,7 +22273,7 @@
         <v>94</v>
       </c>
       <c r="F283" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G283" t="s">
         <v>33</v>
@@ -22315,7 +22318,7 @@
         <v>100</v>
       </c>
       <c r="Z283">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB283">
         <v>0</v>
@@ -22335,7 +22338,7 @@
         <v>94</v>
       </c>
       <c r="F284" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G284" t="s">
         <v>33</v>
@@ -22380,7 +22383,7 @@
         <v>100</v>
       </c>
       <c r="Z284">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB284">
         <v>0</v>
@@ -22400,7 +22403,7 @@
         <v>94</v>
       </c>
       <c r="F285" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G285" t="s">
         <v>33</v>
@@ -22445,7 +22448,7 @@
         <v>100</v>
       </c>
       <c r="Z285">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB285">
         <v>0</v>
@@ -22465,7 +22468,7 @@
         <v>94</v>
       </c>
       <c r="F286" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G286" t="s">
         <v>33</v>
@@ -22510,7 +22513,7 @@
         <v>100</v>
       </c>
       <c r="Z286">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB286">
         <v>0</v>
@@ -22530,7 +22533,7 @@
         <v>94</v>
       </c>
       <c r="F287" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G287" t="s">
         <v>33</v>
@@ -22575,7 +22578,7 @@
         <v>100</v>
       </c>
       <c r="Z287">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB287">
         <v>0</v>
@@ -22595,7 +22598,7 @@
         <v>94</v>
       </c>
       <c r="F288" t="s">
-        <v>71</v>
+        <v>1363</v>
       </c>
       <c r="G288" t="s">
         <v>33</v>
@@ -22640,7 +22643,7 @@
         <v>100</v>
       </c>
       <c r="Z288">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB288">
         <v>0</v>

</xml_diff>